<commit_message>
Update Cart test cases
</commit_message>
<xml_diff>
--- a/Cartpage_test_cases.xlsx
+++ b/Cartpage_test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinee_nemade\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shopizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E17A4F-DC31-45A7-B420-3BDF9E67DE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253E8ADC-1CFE-41C7-B787-90D0B3DFD50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
   <si>
     <t>Sc_id</t>
   </si>
@@ -362,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -422,13 +422,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,15 +717,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="33.6328125" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
     <col min="3" max="3" width="33.7265625" customWidth="1"/>
     <col min="4" max="4" width="46.36328125" customWidth="1"/>
     <col min="5" max="5" width="48.453125" customWidth="1"/>
@@ -755,13 +761,18 @@
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
+      <c r="E2" s="24" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="20"/>
       <c r="D3" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="14" t="s">
@@ -770,6 +781,7 @@
     </row>
     <row r="5" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D5" s="16"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -783,6 +795,9 @@
       </c>
       <c r="D6" s="14" t="s">
         <v>56</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -790,7 +805,9 @@
       <c r="D7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="18"/>
@@ -813,12 +830,16 @@
       <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
+      <c r="E10" s="24" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="18"/>
       <c r="D11" s="14" t="s">
         <v>57</v>
       </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" s="14" t="s">
@@ -840,6 +861,9 @@
       </c>
       <c r="D14" s="14" t="s">
         <v>56</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -848,6 +872,7 @@
       <c r="D15" s="14" t="s">
         <v>57</v>
       </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="18"/>
@@ -855,12 +880,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="23" t="s">
         <v>67</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -869,20 +894,27 @@
       <c r="D18" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="17"/>
       <c r="C19" s="18"/>
       <c r="D19" s="14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D20" s="14" t="s">
         <v>58</v>
       </c>
     </row>
+    <row r="21" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="C18:C19"/>
@@ -899,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -950,14 +982,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="2">
@@ -982,21 +1014,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="18"/>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
+    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="20"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="21" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E4" s="23"/>
+      <c r="B4" s="9"/>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
@@ -1059,7 +1093,7 @@
       <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="21"/>
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1081,7 +1115,7 @@
       <c r="B10" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="2">
@@ -1090,8 +1124,8 @@
       <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>29</v>
+      <c r="F10" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>31</v>
@@ -1115,7 +1149,7 @@
       <c r="E11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1123,7 +1157,7 @@
         <v>37</v>
       </c>
       <c r="E12" s="17"/>
-      <c r="F12" s="23"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1167,7 +1201,7 @@
       <c r="F15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="22" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="11" t="s">
@@ -1189,7 +1223,7 @@
       <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
@@ -1201,7 +1235,7 @@
       <c r="E17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
@@ -1227,11 +1261,11 @@
       <c r="D19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="23" t="s">
-        <v>29</v>
+      <c r="F19" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>52</v>
@@ -1250,21 +1284,25 @@
       <c r="B20" s="18"/>
       <c r="C20" s="17"/>
       <c r="E20" s="17"/>
-      <c r="F20" s="23"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="23"/>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -1284,8 +1322,9 @@
       <c r="D23" s="2">
         <v>1</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>63</v>
+      <c r="E23" s="9" t="str">
+        <f>$E$27</f>
+        <v>Add items in the cart</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>65</v>
@@ -1409,19 +1448,7 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="G19:G20"/>
@@ -1435,9 +1462,21 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F21"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1445,6 +1484,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F4261C012905A7429EEAE0175F0B308C" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a1668bd45395aa4e7106fcf958f3064b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9465699d-b859-4ad6-ab8c-507a684d99d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f77472e7f07b26b0133d681acc3c98c" ns2:_="">
     <xsd:import namespace="9465699d-b859-4ad6-ab8c-507a684d99d6"/>
@@ -1608,12 +1653,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1624,6 +1663,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5E8A97-2FC6-4915-86D4-7EFA9EC0D8AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1641,15 +1689,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1CA316B-A5FF-4AE2-9421-20955EA2F4E1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adding changes in cart test cases
</commit_message>
<xml_diff>
--- a/Cartpage_test_cases.xlsx
+++ b/Cartpage_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shopizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253E8ADC-1CFE-41C7-B787-90D0B3DFD50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974CF594-EEDC-466C-8A52-DD886DF39CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
   <si>
     <t>Sc_id</t>
   </si>
@@ -362,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -410,6 +410,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -422,20 +434,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,7 +729,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -755,18 +764,18 @@
       <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="20"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="14" t="s">
         <v>57</v>
       </c>
@@ -790,7 +799,7 @@
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="14" t="s">
@@ -801,7 +810,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="18"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="14" t="s">
         <v>57</v>
       </c>
@@ -810,7 +819,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="18"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="14" t="s">
         <v>58</v>
       </c>
@@ -824,18 +833,18 @@
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="18"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="14" t="s">
         <v>57</v>
       </c>
@@ -853,29 +862,29 @@
       <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="22" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="14" t="s">
         <v>57</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="18"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="14" t="s">
         <v>58</v>
       </c>
@@ -885,22 +894,22 @@
       <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="23" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="18" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="14" t="s">
         <v>57</v>
       </c>
@@ -929,10 +938,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B32" sqref="B32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,10 +995,10 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="2">
@@ -1001,7 +1010,7 @@
       <c r="F2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="23" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1015,468 +1024,469 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="20"/>
-      <c r="C3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:10" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C7" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="20"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="2">
+    <row r="8" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="24"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="9"/>
-      <c r="C8" s="1" t="s">
+      <c r="G8" s="24"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="9"/>
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="E9" s="26"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C10" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C12" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G12" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="18"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="2">
+    <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="22"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C12" s="1" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D13" s="2">
+      <c r="E14" s="21"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="C15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="2">
         <v>3</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C17" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D17" s="2">
         <v>1</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G17" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="18"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="22"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="2">
         <v>2</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C17" s="1" t="s">
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D19" s="2">
         <v>3</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="22"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C20" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B22" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C22" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D22" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E22" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="18"/>
-      <c r="C20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="1" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="22"/>
+      <c r="C23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="2">
-        <v>2</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="9" t="str">
-        <f>$E$27</f>
-        <v>Add items in the cart</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="18"/>
-      <c r="C24" s="17"/>
       <c r="D24" s="2">
         <v>2</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C25" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="16"/>
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="1:10" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>63</v>
+      <c r="E27" s="9" t="str">
+        <f>$E$32</f>
+        <v>Add items in the cart</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J27" s="19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="18"/>
-      <c r="C28" s="17"/>
+        <v>13</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="22"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="2">
         <v>2</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="21"/>
+    </row>
+    <row r="30" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C30" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B33" s="22"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="J28" s="18"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C29" s="10" t="s">
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="J33" s="22"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
+      <c r="E34" s="21"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="J34" s="22"/>
+    </row>
+    <row r="35" spans="2:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C35" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="19"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="J32:J34"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E24:E25"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="G22:G23"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="E28:E29"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1484,9 +1494,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1654,19 +1667,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1CA316B-A5FF-4AE2-9421-20955EA2F4E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1690,9 +1699,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1CA316B-A5FF-4AE2-9421-20955EA2F4E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding all the updated test cases
</commit_message>
<xml_diff>
--- a/Cartpage_test_cases.xlsx
+++ b/Cartpage_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shopizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974CF594-EEDC-466C-8A52-DD886DF39CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9968110-67F4-4828-B7F2-8D1083F072A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
   <si>
     <t>Sc_id</t>
   </si>
@@ -266,6 +266,15 @@
   </si>
   <si>
     <t>Disounted price should get displayed as total amount</t>
+  </si>
+  <si>
+    <t>Automate</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -419,6 +428,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -434,17 +446,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,7 +773,7 @@
       <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -775,7 +784,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="24"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="14" t="s">
         <v>57</v>
       </c>
@@ -799,7 +808,7 @@
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="14" t="s">
@@ -810,7 +819,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="14" t="s">
         <v>57</v>
       </c>
@@ -819,7 +828,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="14" t="s">
         <v>58</v>
       </c>
@@ -833,7 +842,7 @@
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="23" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="14" t="s">
@@ -844,7 +853,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="14" t="s">
         <v>57</v>
       </c>
@@ -862,10 +871,10 @@
       <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="23" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="14" t="s">
@@ -876,15 +885,15 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="14" t="s">
         <v>57</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="22"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="14" t="s">
         <v>58</v>
       </c>
@@ -894,10 +903,10 @@
       <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="24" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="14" t="s">
@@ -908,8 +917,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="14" t="s">
         <v>57</v>
       </c>
@@ -938,555 +947,580 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:B33"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="2"/>
-    <col min="10" max="10" width="20.453125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="9.1796875" style="2"/>
+    <col min="2" max="2" width="18.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="2"/>
+    <col min="11" max="11" width="20.453125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="24"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="2">
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="25"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="22"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="9"/>
-      <c r="C4" t="s">
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C4" s="9"/>
+      <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="26"/>
-    </row>
-    <row r="5" spans="1:10" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="16" t="s">
+      <c r="F4" s="26"/>
+    </row>
+    <row r="5" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="D5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="19"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" s="9"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="C7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="H7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="2">
+    <row r="8" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="25"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="9"/>
-      <c r="C9" s="1" t="s">
+      <c r="H8" s="25"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C9" s="9"/>
+      <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="1:10" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C10" s="16" t="s">
+      <c r="F9" s="26"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="D10" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" s="9"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="D12" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="H12" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="22"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="2">
+    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="23"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="2">
         <v>2</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="22"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="22"/>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="C15" s="14" t="s">
+      <c r="F14" s="22"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="D15" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>3</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="C17" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="D17" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="H17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B18" s="22"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C18" s="23"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="2">
         <v>2</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C19" s="1" t="s">
+      <c r="H18" s="28"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C20" s="28" t="s">
+      <c r="H19" s="28"/>
+    </row>
+    <row r="20" spans="1:11" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="D20" s="20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="16"/>
-    </row>
-    <row r="22" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="C22" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="D22" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E22" s="2">
         <v>1</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="F22" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="H22" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="22"/>
-      <c r="C23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="G23" s="22"/>
-    </row>
-    <row r="24" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="2">
+      <c r="E24" s="2">
         <v>2</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="F24" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C25" s="28" t="s">
+    <row r="25" spans="1:11" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="D25" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="16"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="1:10" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="27"/>
+    </row>
+    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="16"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="C27" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="D27" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="2">
+      <c r="E27" s="2">
         <v>1</v>
       </c>
-      <c r="E27" s="9" t="str">
-        <f>$E$32</f>
+      <c r="F27" s="9" t="str">
+        <f>$F$32</f>
         <v>Add items in the cart</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="H27" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="22"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="2">
+    <row r="28" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="23"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="2">
         <v>2</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="F28" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C29" s="1" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="21"/>
-    </row>
-    <row r="30" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C30" s="28" t="s">
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:11" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="D30" s="20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="16"/>
-    </row>
-    <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="C32" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="D32" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="2">
+      <c r="E32" s="2">
         <v>1</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G32" s="23" t="s">
+      <c r="H32" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="23" t="s">
+      <c r="I32" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J32" s="23" t="s">
+      <c r="K32" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B33" s="22"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="2">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C33" s="23"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="2">
         <v>2</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="F33" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="J33" s="22"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C34" s="10" t="s">
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="K33" s="23"/>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="21"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="J34" s="22"/>
-    </row>
-    <row r="35" spans="2:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C35" s="28" t="s">
+      <c r="F34" s="22"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="K34" s="23"/>
+    </row>
+    <row r="35" spans="3:11" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="D35" s="20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="19"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
+    <row r="36" spans="3:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="19"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B54" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="F33:F34"/>
     <mergeCell ref="H32:H34"/>
-    <mergeCell ref="J32:J34"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="K32:K34"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1494,12 +1528,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1667,15 +1698,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1CA316B-A5FF-4AE2-9421-20955EA2F4E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1699,10 +1734,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1CA316B-A5FF-4AE2-9421-20955EA2F4E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>